<commit_message>
Updates pinout to avoid TXD, since it flickers on start
</commit_message>
<xml_diff>
--- a/designdiagrams/Relay and Pin Layout.xlsx
+++ b/designdiagrams/Relay and Pin Layout.xlsx
@@ -20,7 +20,6 @@
     <sheet name="ADC Channels" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1229,7 +1228,7 @@
   <dimension ref="A1:BF22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,9 +1877,6 @@
       <c r="H6" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="L6">
         <f t="shared" si="11"/>
         <v>4</v>
@@ -2521,6 +2517,9 @@
       </c>
       <c r="H11" t="s">
         <v>61</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
Updates layout and diagram for correct 3-way valve wiring
</commit_message>
<xml_diff>
--- a/designdiagrams/Relay and Pin Layout.xlsx
+++ b/designdiagrams/Relay and Pin Layout.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomatedBrewery\designdiagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3075" windowHeight="3795" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3075" windowHeight="3795" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Relays" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="RTD Pins" sheetId="5" r:id="rId5"/>
     <sheet name="ADC Channels" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="206">
   <si>
     <t>Relay</t>
   </si>
@@ -541,9 +541,6 @@
     <t>RTD Color</t>
   </si>
   <si>
-    <t>Valve Color</t>
-  </si>
-  <si>
     <t>Gold/Bare</t>
   </si>
   <si>
@@ -641,12 +638,21 @@
   </si>
   <si>
     <t>mosiPin / SDI</t>
+  </si>
+  <si>
+    <t>2 Way Valve Color</t>
+  </si>
+  <si>
+    <t>3 Way Valve Color</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -994,7 +1000,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1260,7 +1266,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="L1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1271,7 +1277,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="Y1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -1282,7 +1288,7 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AL1" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
@@ -1292,7 +1298,7 @@
       <c r="AR1" s="2"/>
       <c r="AS1" s="2"/>
       <c r="AX1" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
@@ -1328,13 +1334,13 @@
         <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L2" t="s">
         <v>7</v>
       </c>
       <c r="M2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N2" t="s">
         <v>8</v>
@@ -1346,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="R2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S2" t="s">
         <v>8</v>
@@ -1355,16 +1361,16 @@
         <v>9</v>
       </c>
       <c r="U2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="X2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Y2" t="s">
         <v>7</v>
       </c>
       <c r="Z2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA2" t="s">
         <v>8</v>
@@ -1376,7 +1382,7 @@
         <v>7</v>
       </c>
       <c r="AE2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AF2" t="s">
         <v>8</v>
@@ -1385,16 +1391,16 @@
         <v>9</v>
       </c>
       <c r="AH2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AK2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AL2" t="s">
         <v>7</v>
       </c>
       <c r="AM2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AN2" t="s">
         <v>8</v>
@@ -1403,7 +1409,7 @@
         <v>9</v>
       </c>
       <c r="AP2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AQ2" t="s">
         <v>7</v>
@@ -1415,16 +1421,16 @@
         <v>9</v>
       </c>
       <c r="AT2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AW2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AX2" t="s">
         <v>7</v>
       </c>
       <c r="AY2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AZ2" t="s">
         <v>8</v>
@@ -1433,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="BB2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BC2" t="s">
         <v>7</v>
@@ -1445,7 +1451,7 @@
         <v>9</v>
       </c>
       <c r="BF2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
@@ -1713,7 +1719,7 @@
         <v>71</v>
       </c>
       <c r="BE4" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
@@ -1810,7 +1816,7 @@
         <v>GPB2</v>
       </c>
       <c r="AO5" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AP5">
         <v>5</v>
@@ -1837,7 +1843,7 @@
         <v>GPB2</v>
       </c>
       <c r="BA5" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BB5">
         <v>5</v>
@@ -2012,7 +2018,7 @@
         <v>58</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L7">
         <f t="shared" si="11"/>
@@ -2519,7 +2525,7 @@
         <v>61</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>160</v>
@@ -3513,7 +3519,7 @@
         <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3562,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3576,7 +3582,7 @@
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>167</v>
       </c>
@@ -3587,73 +3593,85 @@
         <v>169</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
         <v>171</v>
       </c>
-      <c r="C2" t="s">
-        <v>172</v>
-      </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="G2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="G3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
-        <v>179</v>
+        <v>178</v>
+      </c>
+      <c r="G4" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3676,35 +3694,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" t="s">
         <v>184</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>185</v>
-      </c>
-      <c r="D1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -3718,7 +3736,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3732,7 +3750,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3746,7 +3764,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -3776,7 +3794,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -3793,16 +3811,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" t="s">
         <v>184</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>185</v>
-      </c>
-      <c r="D2" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>